<commit_message>
- update excel, html - performed some EDA
</commit_message>
<xml_diff>
--- a/data/SVT_Discography.xlsx
+++ b/data/SVT_Discography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hortenciahernandez/Documents/Random Tests and Projects/Mini Project - 17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A00C69F-40F4-0249-8D77-B16B3D4ABDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2622C0-D241-1A4C-8658-C402D1CF0CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="600" windowWidth="28420" windowHeight="17380" xr2:uid="{D58EBB2E-1547-AB4F-B2D7-20A16C41583F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="463">
   <si>
     <t>Song</t>
   </si>
@@ -1831,8 +1831,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H303" sqref="H303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2184,7 +2184,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -4100,6 +4100,9 @@
       </c>
       <c r="G99" t="s">
         <v>460</v>
+      </c>
+      <c r="H99" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>